<commit_message>
Dynamic pricing - update aggregators tests
</commit_message>
<xml_diff>
--- a/AggregatorsData.xlsx
+++ b/AggregatorsData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="228">
   <si>
     <t>0</t>
   </si>
@@ -74,16 +74,16 @@
         <u val="single"/>
         <sz val="12"/>
         <color indexed="9"/>
-        <rFont val="Helvetica"/>
+        <rFont val="Calibri"/>
       </rPr>
-      <t>http://e1a-eswls-devm-01.es-dte.co.uk:7012/ibisservice/ibisservice</t>
+      <t>http://e1a-eswls-devi-01.es-dte.co.uk:7012/ibisservice/ibisservice</t>
     </r>
   </si>
   <si>
-    <t>m</t>
+    <t>i</t>
   </si>
   <si>
-    <t>chrome</t>
+    <t>firefox</t>
   </si>
   <si>
     <t>Table 1</t>
@@ -278,7 +278,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>SW</t>
+      <t>EM</t>
     </r>
   </si>
   <si>
@@ -584,7 +584,7 @@
     <t>MSM</t>
   </si>
   <si>
-    <t>EH</t>
+    <t>SH</t>
   </si>
   <si>
     <t>107</t>
@@ -692,6 +692,27 @@
     <t>Security Code</t>
   </si>
   <si>
+    <t>DebitAccountHolder (Y/N)</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>SortCodePart1</t>
+  </si>
+  <si>
+    <t>SortCodePart2</t>
+  </si>
+  <si>
+    <t>SortCodePart3</t>
+  </si>
+  <si>
+    <t>Account number</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
@@ -699,6 +720,15 @@
   </si>
   <si>
     <t>4539792000000004</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AutomationMan</t>
+  </si>
+  <si>
+    <t>United Test Bank of Dosh</t>
   </si>
 </sst>
 </file>
@@ -708,7 +738,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -786,12 +816,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="9"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -833,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1229,6 +1253,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="17"/>
       </left>
       <right style="thin">
@@ -1398,7 +1437,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1450,16 +1489,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1519,17 +1558,17 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1537,37 +1576,40 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1607,15 +1649,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>6347</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>178685</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>89577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4354074</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>153446</xdr:rowOff>
+      <xdr:colOff>4347727</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>115138</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1624,7 +1666,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6347" y="826385"/>
+          <a:off x="-19050" y="1169077"/>
           <a:ext cx="4347727" cy="1765462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2205,15 +2247,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>538938</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>118369</xdr:rowOff>
+      <xdr:colOff>557989</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>667560</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>132644</xdr:rowOff>
+      <xdr:colOff>686610</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>152541</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2222,8 +2264,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1783538" y="118369"/>
-          <a:ext cx="6351623" cy="18882684"/>
+          <a:off x="1802589" y="1753708"/>
+          <a:ext cx="6351622" cy="18882684"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8464,14 +8506,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>21182</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38396</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>534952</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>195333</xdr:rowOff>
+      <xdr:colOff>877852</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>189687</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8480,8 +8522,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="2331312"/>
-          <a:ext cx="1779554" cy="1385732"/>
+          <a:off x="-19051" y="1517946"/>
+          <a:ext cx="2122454" cy="1385732"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8938,15 +8980,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>896620</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>149645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1027896</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>6648</xdr:rowOff>
+      <xdr:colOff>937725</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>14687</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8955,8 +8997,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2141220" y="-612464"/>
-          <a:ext cx="6354277" cy="22913664"/>
+          <a:off x="2051050" y="1421550"/>
+          <a:ext cx="6354276" cy="22913664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16576,15 +16618,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>20319</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>21686</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>43658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>845689</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>85983</xdr:rowOff>
+      <xdr:colOff>825369</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>96524</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16593,8 +16635,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20319" y="2331816"/>
-          <a:ext cx="825370" cy="670088"/>
+          <a:off x="-19051" y="1938498"/>
+          <a:ext cx="825371" cy="670087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -35759,7 +35801,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -35771,7 +35813,14 @@
     <col min="4" max="4" width="16.3516" style="39" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="39" customWidth="1"/>
     <col min="6" max="6" width="16.3516" style="39" customWidth="1"/>
-    <col min="7" max="256" width="16.3516" style="39" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="39" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="39" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="39" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="39" customWidth="1"/>
+    <col min="11" max="11" width="16.3516" style="39" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="39" customWidth="1"/>
+    <col min="13" max="13" width="16.3516" style="39" customWidth="1"/>
+    <col min="14" max="256" width="16.3516" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -35783,110 +35832,215 @@
       <c r="D1" s="41"/>
       <c r="E1" s="41"/>
       <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" t="s" s="43">
+      <c r="A2" t="s" s="44">
         <v>209</v>
       </c>
-      <c r="B2" t="s" s="44">
+      <c r="B2" t="s" s="45">
         <v>210</v>
       </c>
-      <c r="C2" t="s" s="44">
+      <c r="C2" t="s" s="45">
         <v>211</v>
       </c>
-      <c r="D2" t="s" s="44">
+      <c r="D2" t="s" s="45">
         <v>212</v>
       </c>
-      <c r="E2" t="s" s="44">
+      <c r="E2" t="s" s="45">
         <v>213</v>
       </c>
       <c r="F2" t="s" s="45">
         <v>214</v>
       </c>
+      <c r="G2" t="s" s="45">
+        <v>215</v>
+      </c>
+      <c r="H2" t="s" s="45">
+        <v>216</v>
+      </c>
+      <c r="I2" t="s" s="45">
+        <v>217</v>
+      </c>
+      <c r="J2" t="s" s="45">
+        <v>218</v>
+      </c>
+      <c r="K2" t="s" s="46">
+        <v>219</v>
+      </c>
+      <c r="L2" t="s" s="44">
+        <v>220</v>
+      </c>
+      <c r="M2" t="s" s="46">
+        <v>221</v>
+      </c>
     </row>
     <row r="3" ht="16.55" customHeight="1">
-      <c r="A3" t="s" s="46">
-        <v>215</v>
+      <c r="A3" t="s" s="47">
+        <v>222</v>
       </c>
       <c r="B3" t="s" s="23">
-        <v>216</v>
+        <v>223</v>
       </c>
-      <c r="C3" t="s" s="47">
-        <v>217</v>
+      <c r="C3" t="s" s="48">
+        <v>224</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="49">
         <v>12</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="49">
         <v>2022</v>
       </c>
       <c r="F3" s="49">
         <v>444</v>
       </c>
+      <c r="G3" t="s" s="24">
+        <v>225</v>
+      </c>
+      <c r="H3" t="s" s="24">
+        <v>226</v>
+      </c>
+      <c r="I3" s="49">
+        <v>40</v>
+      </c>
+      <c r="J3" s="49">
+        <v>27</v>
+      </c>
+      <c r="K3" s="49">
+        <v>15</v>
+      </c>
+      <c r="L3" s="49">
+        <v>22859882</v>
+      </c>
+      <c r="M3" t="s" s="50">
+        <v>227</v>
+      </c>
     </row>
     <row r="4" ht="16.35" customHeight="1">
-      <c r="A4" s="50"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
-      <c r="F4" s="51"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="52"/>
     </row>
     <row r="5" ht="16.35" customHeight="1">
-      <c r="A5" s="50"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
-      <c r="F5" s="51"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" ht="16.35" customHeight="1">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="26"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
-      <c r="F6" s="51"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="52"/>
     </row>
     <row r="7" ht="16.35" customHeight="1">
-      <c r="A7" s="50"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="52"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
-      <c r="F7" s="51"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="52"/>
     </row>
     <row r="8" ht="16.35" customHeight="1">
-      <c r="A8" s="50"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="26"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="51"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="52"/>
     </row>
     <row r="9" ht="16.35" customHeight="1">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="26"/>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
-      <c r="F9" s="51"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="52"/>
     </row>
     <row r="10" ht="16.35" customHeight="1">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
-      <c r="F10" s="51"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" ht="16.3" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added aggregator tests for each brand
</commit_message>
<xml_diff>
--- a/AggregatorsData.xlsx
+++ b/AggregatorsData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
   <si>
     <t>0</t>
   </si>
@@ -407,6 +407,26 @@
     <t>Wiltshire</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>SW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>FC</t>
+    </r>
+  </si>
+  <si>
     <t>specialTermsFlag (true/false)</t>
   </si>
   <si>
@@ -584,7 +604,7 @@
     <t>MSM</t>
   </si>
   <si>
-    <t>SH</t>
+    <t>EH</t>
   </si>
   <si>
     <t>107</t>
@@ -672,6 +692,9 @@
   </si>
   <si>
     <t xml:space="preserve">false  </t>
+  </si>
+  <si>
+    <t>SH</t>
   </si>
   <si>
     <t>Card Type</t>
@@ -857,7 +880,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1050,6 +1073,51 @@
       </right>
       <top style="thin">
         <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
         <color indexed="15"/>
@@ -1437,7 +1505,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1513,16 +1581,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1540,76 +1608,85 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1650,14 +1727,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>89577</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4347727</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>115138</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1666,8 +1743,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="1169077"/>
-          <a:ext cx="4347727" cy="1765462"/>
+          <a:off x="-19051" y="1053938"/>
+          <a:ext cx="4347728" cy="1765462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2247,15 +2324,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>557989</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66513</xdr:rowOff>
+      <xdr:colOff>467818</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>686610</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>152541</xdr:rowOff>
+      <xdr:colOff>596440</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>83273</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2264,8 +2341,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1802589" y="1753708"/>
-          <a:ext cx="6351622" cy="18882684"/>
+          <a:off x="1712418" y="1482510"/>
+          <a:ext cx="6351623" cy="18882684"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8506,14 +8583,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38396</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>118152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>877852</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>189687</xdr:rowOff>
+      <xdr:colOff>915952</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>90374</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8522,8 +8599,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="1517946"/>
-          <a:ext cx="2122454" cy="1385732"/>
+          <a:off x="-19051" y="2630212"/>
+          <a:ext cx="2160554" cy="1385732"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8980,14 +9057,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>149645</xdr:rowOff>
+      <xdr:colOff>980440</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>155360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>937725</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:colOff>1111716</xdr:colOff>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>14687</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -8997,7 +9074,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2051050" y="1421550"/>
+          <a:off x="2225040" y="1219620"/>
           <a:ext cx="6354276" cy="22913664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16619,14 +16696,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>43658</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>825369</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>96524</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133113</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16635,8 +16712,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="1938498"/>
-          <a:ext cx="825371" cy="670087"/>
+          <a:off x="-19051" y="2580876"/>
+          <a:ext cx="825370" cy="670088"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18735,562 +18812,802 @@
       </c>
     </row>
     <row r="4" ht="16.35" customHeight="1">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27"/>
-      <c r="AX4" s="27"/>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="27"/>
-      <c r="BD4" s="27"/>
-      <c r="BE4" s="27"/>
-      <c r="BF4" s="27"/>
-      <c r="BG4" s="27"/>
-      <c r="BH4" s="27"/>
+      <c r="A4" t="s" s="22">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s" s="23">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s" s="24">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s" s="24">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s" s="24">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s" s="24">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s" s="24">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s" s="24">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s" s="24">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s" s="24">
+        <v>86</v>
+      </c>
+      <c r="M4" t="s" s="24">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s" s="24">
+        <v>87</v>
+      </c>
+      <c r="O4" t="s" s="24">
+        <v>88</v>
+      </c>
+      <c r="P4" t="s" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s" s="24">
+        <v>89</v>
+      </c>
+      <c r="R4" t="s" s="24">
+        <v>89</v>
+      </c>
+      <c r="S4" t="s" s="24">
+        <v>90</v>
+      </c>
+      <c r="T4" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="U4" t="s" s="24">
+        <v>91</v>
+      </c>
+      <c r="V4" t="s" s="24">
+        <v>92</v>
+      </c>
+      <c r="W4" t="s" s="24">
+        <v>93</v>
+      </c>
+      <c r="X4" t="s" s="24">
+        <v>94</v>
+      </c>
+      <c r="Y4" t="s" s="24">
+        <v>95</v>
+      </c>
+      <c r="Z4" t="s" s="24">
+        <v>96</v>
+      </c>
+      <c r="AA4" t="s" s="24">
+        <v>97</v>
+      </c>
+      <c r="AB4" t="s" s="24">
+        <v>98</v>
+      </c>
+      <c r="AC4" t="s" s="24">
+        <v>99</v>
+      </c>
+      <c r="AD4" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="AE4" t="s" s="24">
+        <v>100</v>
+      </c>
+      <c r="AF4" t="s" s="24">
+        <v>100</v>
+      </c>
+      <c r="AG4" t="s" s="24">
+        <v>101</v>
+      </c>
+      <c r="AH4" t="s" s="24">
+        <v>102</v>
+      </c>
+      <c r="AI4" t="s" s="24">
+        <v>103</v>
+      </c>
+      <c r="AJ4" t="s" s="24">
+        <v>104</v>
+      </c>
+      <c r="AK4" t="s" s="24">
+        <v>105</v>
+      </c>
+      <c r="AL4" t="s" s="24">
+        <v>106</v>
+      </c>
+      <c r="AM4" t="s" s="24">
+        <v>107</v>
+      </c>
+      <c r="AN4" t="s" s="24">
+        <v>4</v>
+      </c>
+      <c r="AO4" t="s" s="24">
+        <v>108</v>
+      </c>
+      <c r="AP4" t="s" s="24">
+        <v>108</v>
+      </c>
+      <c r="AQ4" t="s" s="24">
+        <v>109</v>
+      </c>
+      <c r="AR4" t="s" s="24">
+        <v>1</v>
+      </c>
+      <c r="AS4" t="s" s="24">
+        <v>110</v>
+      </c>
+      <c r="AT4" t="s" s="24">
+        <v>111</v>
+      </c>
+      <c r="AU4" t="s" s="24">
+        <v>112</v>
+      </c>
+      <c r="AV4" t="s" s="24">
+        <v>113</v>
+      </c>
+      <c r="AW4" t="s" s="24">
+        <v>114</v>
+      </c>
+      <c r="AX4" t="s" s="24">
+        <v>4</v>
+      </c>
+      <c r="AY4" t="s" s="24">
+        <v>115</v>
+      </c>
+      <c r="AZ4" t="s" s="24">
+        <v>116</v>
+      </c>
+      <c r="BA4" t="s" s="24">
+        <v>90</v>
+      </c>
+      <c r="BB4" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="BC4" t="s" s="24">
+        <v>90</v>
+      </c>
+      <c r="BD4" t="s" s="24">
+        <v>90</v>
+      </c>
+      <c r="BE4" t="s" s="24">
+        <v>88</v>
+      </c>
+      <c r="BF4" t="s" s="24">
+        <v>117</v>
+      </c>
+      <c r="BG4" t="s" s="24">
+        <v>118</v>
+      </c>
+      <c r="BH4" t="s" s="24">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" ht="16.35" customHeight="1">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="27"/>
-      <c r="AM5" s="27"/>
-      <c r="AN5" s="27"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="27"/>
-      <c r="AR5" s="27"/>
-      <c r="AS5" s="27"/>
-      <c r="AT5" s="27"/>
-      <c r="AU5" s="27"/>
-      <c r="AV5" s="27"/>
-      <c r="AW5" s="27"/>
-      <c r="AX5" s="27"/>
-      <c r="AY5" s="27"/>
-      <c r="AZ5" s="27"/>
-      <c r="BA5" s="27"/>
-      <c r="BB5" s="27"/>
-      <c r="BC5" s="27"/>
-      <c r="BD5" s="27"/>
-      <c r="BE5" s="27"/>
-      <c r="BF5" s="27"/>
-      <c r="BG5" s="27"/>
-      <c r="BH5" s="27"/>
+      <c r="A5" t="s" s="25">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s" s="27">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s" s="27">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s" s="27">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s" s="27">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s" s="27">
+        <v>85</v>
+      </c>
+      <c r="I5" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s" s="27">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s" s="27">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s" s="27">
+        <v>86</v>
+      </c>
+      <c r="M5" t="s" s="27">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s" s="27">
+        <v>87</v>
+      </c>
+      <c r="O5" t="s" s="27">
+        <v>88</v>
+      </c>
+      <c r="P5" t="s" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s" s="27">
+        <v>89</v>
+      </c>
+      <c r="R5" t="s" s="27">
+        <v>89</v>
+      </c>
+      <c r="S5" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="T5" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="U5" t="s" s="27">
+        <v>91</v>
+      </c>
+      <c r="V5" t="s" s="27">
+        <v>92</v>
+      </c>
+      <c r="W5" t="s" s="27">
+        <v>93</v>
+      </c>
+      <c r="X5" t="s" s="27">
+        <v>94</v>
+      </c>
+      <c r="Y5" t="s" s="27">
+        <v>95</v>
+      </c>
+      <c r="Z5" t="s" s="27">
+        <v>96</v>
+      </c>
+      <c r="AA5" t="s" s="27">
+        <v>97</v>
+      </c>
+      <c r="AB5" t="s" s="27">
+        <v>98</v>
+      </c>
+      <c r="AC5" t="s" s="27">
+        <v>99</v>
+      </c>
+      <c r="AD5" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AE5" t="s" s="27">
+        <v>100</v>
+      </c>
+      <c r="AF5" t="s" s="27">
+        <v>100</v>
+      </c>
+      <c r="AG5" t="s" s="27">
+        <v>101</v>
+      </c>
+      <c r="AH5" t="s" s="27">
+        <v>102</v>
+      </c>
+      <c r="AI5" t="s" s="27">
+        <v>103</v>
+      </c>
+      <c r="AJ5" t="s" s="27">
+        <v>104</v>
+      </c>
+      <c r="AK5" t="s" s="27">
+        <v>105</v>
+      </c>
+      <c r="AL5" t="s" s="27">
+        <v>106</v>
+      </c>
+      <c r="AM5" t="s" s="27">
+        <v>107</v>
+      </c>
+      <c r="AN5" t="s" s="27">
+        <v>4</v>
+      </c>
+      <c r="AO5" t="s" s="27">
+        <v>108</v>
+      </c>
+      <c r="AP5" t="s" s="27">
+        <v>108</v>
+      </c>
+      <c r="AQ5" t="s" s="27">
+        <v>109</v>
+      </c>
+      <c r="AR5" t="s" s="27">
+        <v>1</v>
+      </c>
+      <c r="AS5" t="s" s="27">
+        <v>110</v>
+      </c>
+      <c r="AT5" t="s" s="27">
+        <v>111</v>
+      </c>
+      <c r="AU5" t="s" s="27">
+        <v>112</v>
+      </c>
+      <c r="AV5" t="s" s="27">
+        <v>113</v>
+      </c>
+      <c r="AW5" t="s" s="27">
+        <v>114</v>
+      </c>
+      <c r="AX5" t="s" s="27">
+        <v>4</v>
+      </c>
+      <c r="AY5" t="s" s="27">
+        <v>115</v>
+      </c>
+      <c r="AZ5" t="s" s="27">
+        <v>116</v>
+      </c>
+      <c r="BA5" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="BB5" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="BC5" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="BD5" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="BE5" t="s" s="27">
+        <v>88</v>
+      </c>
+      <c r="BF5" t="s" s="27">
+        <v>117</v>
+      </c>
+      <c r="BG5" t="s" s="27">
+        <v>118</v>
+      </c>
+      <c r="BH5" t="s" s="27">
+        <v>119</v>
+      </c>
     </row>
     <row r="6" ht="16.35" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="27"/>
-      <c r="AF6" s="27"/>
-      <c r="AG6" s="27"/>
-      <c r="AH6" s="27"/>
-      <c r="AI6" s="27"/>
-      <c r="AJ6" s="27"/>
-      <c r="AK6" s="27"/>
-      <c r="AL6" s="27"/>
-      <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="27"/>
-      <c r="AQ6" s="27"/>
-      <c r="AR6" s="27"/>
-      <c r="AS6" s="27"/>
-      <c r="AT6" s="27"/>
-      <c r="AU6" s="27"/>
-      <c r="AV6" s="27"/>
-      <c r="AW6" s="27"/>
-      <c r="AX6" s="27"/>
-      <c r="AY6" s="27"/>
-      <c r="AZ6" s="27"/>
-      <c r="BA6" s="27"/>
-      <c r="BB6" s="27"/>
-      <c r="BC6" s="27"/>
-      <c r="BD6" s="27"/>
-      <c r="BE6" s="27"/>
-      <c r="BF6" s="27"/>
-      <c r="BG6" s="27"/>
-      <c r="BH6" s="27"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="30"/>
+      <c r="AM6" s="30"/>
+      <c r="AN6" s="30"/>
+      <c r="AO6" s="30"/>
+      <c r="AP6" s="30"/>
+      <c r="AQ6" s="30"/>
+      <c r="AR6" s="30"/>
+      <c r="AS6" s="30"/>
+      <c r="AT6" s="30"/>
+      <c r="AU6" s="30"/>
+      <c r="AV6" s="30"/>
+      <c r="AW6" s="30"/>
+      <c r="AX6" s="30"/>
+      <c r="AY6" s="30"/>
+      <c r="AZ6" s="30"/>
+      <c r="BA6" s="30"/>
+      <c r="BB6" s="30"/>
+      <c r="BC6" s="30"/>
+      <c r="BD6" s="30"/>
+      <c r="BE6" s="30"/>
+      <c r="BF6" s="30"/>
+      <c r="BG6" s="30"/>
+      <c r="BH6" s="30"/>
     </row>
     <row r="7" ht="16.35" customHeight="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="27"/>
-      <c r="AC7" s="27"/>
-      <c r="AD7" s="27"/>
-      <c r="AE7" s="27"/>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="27"/>
-      <c r="AI7" s="27"/>
-      <c r="AJ7" s="27"/>
-      <c r="AK7" s="27"/>
-      <c r="AL7" s="27"/>
-      <c r="AM7" s="27"/>
-      <c r="AN7" s="27"/>
-      <c r="AO7" s="27"/>
-      <c r="AP7" s="27"/>
-      <c r="AQ7" s="27"/>
-      <c r="AR7" s="27"/>
-      <c r="AS7" s="27"/>
-      <c r="AT7" s="27"/>
-      <c r="AU7" s="27"/>
-      <c r="AV7" s="27"/>
-      <c r="AW7" s="27"/>
-      <c r="AX7" s="27"/>
-      <c r="AY7" s="27"/>
-      <c r="AZ7" s="27"/>
-      <c r="BA7" s="27"/>
-      <c r="BB7" s="27"/>
-      <c r="BC7" s="27"/>
-      <c r="BD7" s="27"/>
-      <c r="BE7" s="27"/>
-      <c r="BF7" s="27"/>
-      <c r="BG7" s="27"/>
-      <c r="BH7" s="27"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="30"/>
+      <c r="AM7" s="30"/>
+      <c r="AN7" s="30"/>
+      <c r="AO7" s="30"/>
+      <c r="AP7" s="30"/>
+      <c r="AQ7" s="30"/>
+      <c r="AR7" s="30"/>
+      <c r="AS7" s="30"/>
+      <c r="AT7" s="30"/>
+      <c r="AU7" s="30"/>
+      <c r="AV7" s="30"/>
+      <c r="AW7" s="30"/>
+      <c r="AX7" s="30"/>
+      <c r="AY7" s="30"/>
+      <c r="AZ7" s="30"/>
+      <c r="BA7" s="30"/>
+      <c r="BB7" s="30"/>
+      <c r="BC7" s="30"/>
+      <c r="BD7" s="30"/>
+      <c r="BE7" s="30"/>
+      <c r="BF7" s="30"/>
+      <c r="BG7" s="30"/>
+      <c r="BH7" s="30"/>
     </row>
     <row r="8" ht="16.35" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="27"/>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="27"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="27"/>
-      <c r="AM8" s="27"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
-      <c r="AS8" s="27"/>
-      <c r="AT8" s="27"/>
-      <c r="AU8" s="27"/>
-      <c r="AV8" s="27"/>
-      <c r="AW8" s="27"/>
-      <c r="AX8" s="27"/>
-      <c r="AY8" s="27"/>
-      <c r="AZ8" s="27"/>
-      <c r="BA8" s="27"/>
-      <c r="BB8" s="27"/>
-      <c r="BC8" s="27"/>
-      <c r="BD8" s="27"/>
-      <c r="BE8" s="27"/>
-      <c r="BF8" s="27"/>
-      <c r="BG8" s="27"/>
-      <c r="BH8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="30"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="30"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="30"/>
+      <c r="AH8" s="30"/>
+      <c r="AI8" s="30"/>
+      <c r="AJ8" s="30"/>
+      <c r="AK8" s="30"/>
+      <c r="AL8" s="30"/>
+      <c r="AM8" s="30"/>
+      <c r="AN8" s="30"/>
+      <c r="AO8" s="30"/>
+      <c r="AP8" s="30"/>
+      <c r="AQ8" s="30"/>
+      <c r="AR8" s="30"/>
+      <c r="AS8" s="30"/>
+      <c r="AT8" s="30"/>
+      <c r="AU8" s="30"/>
+      <c r="AV8" s="30"/>
+      <c r="AW8" s="30"/>
+      <c r="AX8" s="30"/>
+      <c r="AY8" s="30"/>
+      <c r="AZ8" s="30"/>
+      <c r="BA8" s="30"/>
+      <c r="BB8" s="30"/>
+      <c r="BC8" s="30"/>
+      <c r="BD8" s="30"/>
+      <c r="BE8" s="30"/>
+      <c r="BF8" s="30"/>
+      <c r="BG8" s="30"/>
+      <c r="BH8" s="30"/>
     </row>
     <row r="9" ht="16.35" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="27"/>
-      <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="27"/>
-      <c r="AI9" s="27"/>
-      <c r="AJ9" s="27"/>
-      <c r="AK9" s="27"/>
-      <c r="AL9" s="27"/>
-      <c r="AM9" s="27"/>
-      <c r="AN9" s="27"/>
-      <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
-      <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
-      <c r="AS9" s="27"/>
-      <c r="AT9" s="27"/>
-      <c r="AU9" s="27"/>
-      <c r="AV9" s="27"/>
-      <c r="AW9" s="27"/>
-      <c r="AX9" s="27"/>
-      <c r="AY9" s="27"/>
-      <c r="AZ9" s="27"/>
-      <c r="BA9" s="27"/>
-      <c r="BB9" s="27"/>
-      <c r="BC9" s="27"/>
-      <c r="BD9" s="27"/>
-      <c r="BE9" s="27"/>
-      <c r="BF9" s="27"/>
-      <c r="BG9" s="27"/>
-      <c r="BH9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="30"/>
+      <c r="AJ9" s="30"/>
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="30"/>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="30"/>
+      <c r="AO9" s="30"/>
+      <c r="AP9" s="30"/>
+      <c r="AQ9" s="30"/>
+      <c r="AR9" s="30"/>
+      <c r="AS9" s="30"/>
+      <c r="AT9" s="30"/>
+      <c r="AU9" s="30"/>
+      <c r="AV9" s="30"/>
+      <c r="AW9" s="30"/>
+      <c r="AX9" s="30"/>
+      <c r="AY9" s="30"/>
+      <c r="AZ9" s="30"/>
+      <c r="BA9" s="30"/>
+      <c r="BB9" s="30"/>
+      <c r="BC9" s="30"/>
+      <c r="BD9" s="30"/>
+      <c r="BE9" s="30"/>
+      <c r="BF9" s="30"/>
+      <c r="BG9" s="30"/>
+      <c r="BH9" s="30"/>
     </row>
     <row r="10" ht="16.35" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="27"/>
-      <c r="AM10" s="27"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
-      <c r="AR10" s="27"/>
-      <c r="AS10" s="27"/>
-      <c r="AT10" s="27"/>
-      <c r="AU10" s="27"/>
-      <c r="AV10" s="27"/>
-      <c r="AW10" s="27"/>
-      <c r="AX10" s="27"/>
-      <c r="AY10" s="27"/>
-      <c r="AZ10" s="27"/>
-      <c r="BA10" s="27"/>
-      <c r="BB10" s="27"/>
-      <c r="BC10" s="27"/>
-      <c r="BD10" s="27"/>
-      <c r="BE10" s="27"/>
-      <c r="BF10" s="27"/>
-      <c r="BG10" s="27"/>
-      <c r="BH10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="30"/>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30"/>
+      <c r="AO10" s="30"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="30"/>
+      <c r="AR10" s="30"/>
+      <c r="AS10" s="30"/>
+      <c r="AT10" s="30"/>
+      <c r="AU10" s="30"/>
+      <c r="AV10" s="30"/>
+      <c r="AW10" s="30"/>
+      <c r="AX10" s="30"/>
+      <c r="AY10" s="30"/>
+      <c r="AZ10" s="30"/>
+      <c r="BA10" s="30"/>
+      <c r="BB10" s="30"/>
+      <c r="BC10" s="30"/>
+      <c r="BD10" s="30"/>
+      <c r="BE10" s="30"/>
+      <c r="BF10" s="30"/>
+      <c r="BG10" s="30"/>
+      <c r="BH10" s="30"/>
     </row>
     <row r="11" ht="16.35" customHeight="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="27"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="27"/>
-      <c r="AJ11" s="27"/>
-      <c r="AK11" s="27"/>
-      <c r="AL11" s="27"/>
-      <c r="AM11" s="27"/>
-      <c r="AN11" s="27"/>
-      <c r="AO11" s="27"/>
-      <c r="AP11" s="27"/>
-      <c r="AQ11" s="27"/>
-      <c r="AR11" s="27"/>
-      <c r="AS11" s="27"/>
-      <c r="AT11" s="27"/>
-      <c r="AU11" s="27"/>
-      <c r="AV11" s="27"/>
-      <c r="AW11" s="27"/>
-      <c r="AX11" s="27"/>
-      <c r="AY11" s="27"/>
-      <c r="AZ11" s="27"/>
-      <c r="BA11" s="27"/>
-      <c r="BB11" s="27"/>
-      <c r="BC11" s="27"/>
-      <c r="BD11" s="27"/>
-      <c r="BE11" s="27"/>
-      <c r="BF11" s="27"/>
-      <c r="BG11" s="27"/>
-      <c r="BH11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="30"/>
+      <c r="AK11" s="30"/>
+      <c r="AL11" s="30"/>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30"/>
+      <c r="AO11" s="30"/>
+      <c r="AP11" s="30"/>
+      <c r="AQ11" s="30"/>
+      <c r="AR11" s="30"/>
+      <c r="AS11" s="30"/>
+      <c r="AT11" s="30"/>
+      <c r="AU11" s="30"/>
+      <c r="AV11" s="30"/>
+      <c r="AW11" s="30"/>
+      <c r="AX11" s="30"/>
+      <c r="AY11" s="30"/>
+      <c r="AZ11" s="30"/>
+      <c r="BA11" s="30"/>
+      <c r="BB11" s="30"/>
+      <c r="BC11" s="30"/>
+      <c r="BD11" s="30"/>
+      <c r="BE11" s="30"/>
+      <c r="BF11" s="30"/>
+      <c r="BG11" s="30"/>
+      <c r="BH11" s="30"/>
     </row>
     <row r="12" ht="15.9" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="29"/>
-      <c r="AD12" s="29"/>
-      <c r="AE12" s="29"/>
-      <c r="AF12" s="29"/>
-      <c r="AG12" s="29"/>
-      <c r="AH12" s="29"/>
-      <c r="AI12" s="29"/>
-      <c r="AJ12" s="29"/>
-      <c r="AK12" s="29"/>
-      <c r="AL12" s="29"/>
-      <c r="AM12" s="29"/>
-      <c r="AN12" s="29"/>
-      <c r="AO12" s="29"/>
-      <c r="AP12" s="29"/>
-      <c r="AQ12" s="29"/>
-      <c r="AR12" s="29"/>
-      <c r="AS12" s="29"/>
-      <c r="AT12" s="29"/>
-      <c r="AU12" s="29"/>
-      <c r="AV12" s="29"/>
-      <c r="AW12" s="29"/>
-      <c r="AX12" s="29"/>
-      <c r="AY12" s="29"/>
-      <c r="AZ12" s="29"/>
-      <c r="BA12" s="29"/>
-      <c r="BB12" s="29"/>
-      <c r="BC12" s="29"/>
-      <c r="BD12" s="29"/>
-      <c r="BE12" s="29"/>
-      <c r="BF12" s="29"/>
-      <c r="BG12" s="29"/>
-      <c r="BH12" s="30"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
+      <c r="AI12" s="32"/>
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="32"/>
+      <c r="AL12" s="32"/>
+      <c r="AM12" s="32"/>
+      <c r="AN12" s="32"/>
+      <c r="AO12" s="32"/>
+      <c r="AP12" s="32"/>
+      <c r="AQ12" s="32"/>
+      <c r="AR12" s="32"/>
+      <c r="AS12" s="32"/>
+      <c r="AT12" s="32"/>
+      <c r="AU12" s="32"/>
+      <c r="AV12" s="32"/>
+      <c r="AW12" s="32"/>
+      <c r="AX12" s="32"/>
+      <c r="AY12" s="32"/>
+      <c r="AZ12" s="32"/>
+      <c r="BA12" s="32"/>
+      <c r="BB12" s="32"/>
+      <c r="BC12" s="32"/>
+      <c r="BD12" s="32"/>
+      <c r="BE12" s="32"/>
+      <c r="BF12" s="32"/>
+      <c r="BG12" s="32"/>
+      <c r="BH12" s="33"/>
     </row>
     <row r="13" ht="15.9" customHeight="1">
       <c r="A13" s="6"/>
@@ -24873,66 +25190,66 @@
       <c r="BH102" s="13"/>
     </row>
     <row r="103" ht="15.9" customHeight="1">
-      <c r="A103" s="31"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="32"/>
-      <c r="H103" s="32"/>
-      <c r="I103" s="32"/>
-      <c r="J103" s="32"/>
-      <c r="K103" s="32"/>
-      <c r="L103" s="32"/>
-      <c r="M103" s="32"/>
-      <c r="N103" s="32"/>
-      <c r="O103" s="32"/>
-      <c r="P103" s="32"/>
-      <c r="Q103" s="32"/>
-      <c r="R103" s="32"/>
-      <c r="S103" s="32"/>
-      <c r="T103" s="32"/>
-      <c r="U103" s="32"/>
-      <c r="V103" s="32"/>
-      <c r="W103" s="32"/>
-      <c r="X103" s="32"/>
-      <c r="Y103" s="32"/>
-      <c r="Z103" s="32"/>
-      <c r="AA103" s="32"/>
-      <c r="AB103" s="32"/>
-      <c r="AC103" s="32"/>
-      <c r="AD103" s="32"/>
-      <c r="AE103" s="32"/>
-      <c r="AF103" s="32"/>
-      <c r="AG103" s="32"/>
-      <c r="AH103" s="32"/>
-      <c r="AI103" s="32"/>
-      <c r="AJ103" s="32"/>
-      <c r="AK103" s="32"/>
-      <c r="AL103" s="32"/>
-      <c r="AM103" s="32"/>
-      <c r="AN103" s="32"/>
-      <c r="AO103" s="32"/>
-      <c r="AP103" s="32"/>
-      <c r="AQ103" s="32"/>
-      <c r="AR103" s="32"/>
-      <c r="AS103" s="32"/>
-      <c r="AT103" s="32"/>
-      <c r="AU103" s="32"/>
-      <c r="AV103" s="32"/>
-      <c r="AW103" s="32"/>
-      <c r="AX103" s="32"/>
-      <c r="AY103" s="32"/>
-      <c r="AZ103" s="32"/>
-      <c r="BA103" s="32"/>
-      <c r="BB103" s="32"/>
-      <c r="BC103" s="32"/>
-      <c r="BD103" s="32"/>
-      <c r="BE103" s="32"/>
-      <c r="BF103" s="32"/>
-      <c r="BG103" s="32"/>
-      <c r="BH103" s="33"/>
+      <c r="A103" s="34"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="35"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
+      <c r="P103" s="35"/>
+      <c r="Q103" s="35"/>
+      <c r="R103" s="35"/>
+      <c r="S103" s="35"/>
+      <c r="T103" s="35"/>
+      <c r="U103" s="35"/>
+      <c r="V103" s="35"/>
+      <c r="W103" s="35"/>
+      <c r="X103" s="35"/>
+      <c r="Y103" s="35"/>
+      <c r="Z103" s="35"/>
+      <c r="AA103" s="35"/>
+      <c r="AB103" s="35"/>
+      <c r="AC103" s="35"/>
+      <c r="AD103" s="35"/>
+      <c r="AE103" s="35"/>
+      <c r="AF103" s="35"/>
+      <c r="AG103" s="35"/>
+      <c r="AH103" s="35"/>
+      <c r="AI103" s="35"/>
+      <c r="AJ103" s="35"/>
+      <c r="AK103" s="35"/>
+      <c r="AL103" s="35"/>
+      <c r="AM103" s="35"/>
+      <c r="AN103" s="35"/>
+      <c r="AO103" s="35"/>
+      <c r="AP103" s="35"/>
+      <c r="AQ103" s="35"/>
+      <c r="AR103" s="35"/>
+      <c r="AS103" s="35"/>
+      <c r="AT103" s="35"/>
+      <c r="AU103" s="35"/>
+      <c r="AV103" s="35"/>
+      <c r="AW103" s="35"/>
+      <c r="AX103" s="35"/>
+      <c r="AY103" s="35"/>
+      <c r="AZ103" s="35"/>
+      <c r="BA103" s="35"/>
+      <c r="BB103" s="35"/>
+      <c r="BC103" s="35"/>
+      <c r="BD103" s="35"/>
+      <c r="BE103" s="35"/>
+      <c r="BF103" s="35"/>
+      <c r="BG103" s="35"/>
+      <c r="BH103" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -24940,13 +25257,15 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AQ3" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="AQ4" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="AQ5" r:id="rId3" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -24961,91 +25280,91 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="34" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="34" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="34" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="34" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="34" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="34" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="34" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="34" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="34" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="34" customWidth="1"/>
-    <col min="11" max="11" width="16.3516" style="34" customWidth="1"/>
-    <col min="12" max="12" width="16.3516" style="34" customWidth="1"/>
-    <col min="13" max="13" width="16.3516" style="34" customWidth="1"/>
-    <col min="14" max="14" width="16.3516" style="34" customWidth="1"/>
-    <col min="15" max="15" width="16.3516" style="34" customWidth="1"/>
-    <col min="16" max="16" width="16.3516" style="34" customWidth="1"/>
-    <col min="17" max="17" width="16.3516" style="34" customWidth="1"/>
-    <col min="18" max="18" width="16.3516" style="34" customWidth="1"/>
-    <col min="19" max="19" width="16.3516" style="34" customWidth="1"/>
-    <col min="20" max="20" width="16.3516" style="34" customWidth="1"/>
-    <col min="21" max="21" width="16.3516" style="34" customWidth="1"/>
-    <col min="22" max="22" width="16.3516" style="34" customWidth="1"/>
-    <col min="23" max="23" width="16.3516" style="34" customWidth="1"/>
-    <col min="24" max="24" width="16.3516" style="34" customWidth="1"/>
-    <col min="25" max="25" width="16.3516" style="34" customWidth="1"/>
-    <col min="26" max="26" width="16.3516" style="34" customWidth="1"/>
-    <col min="27" max="27" width="16.3516" style="34" customWidth="1"/>
-    <col min="28" max="28" width="16.3516" style="34" customWidth="1"/>
-    <col min="29" max="29" width="16.3516" style="34" customWidth="1"/>
-    <col min="30" max="30" width="16.3516" style="34" customWidth="1"/>
-    <col min="31" max="31" width="16.3516" style="34" customWidth="1"/>
-    <col min="32" max="32" width="16.3516" style="34" customWidth="1"/>
-    <col min="33" max="33" width="16.3516" style="34" customWidth="1"/>
-    <col min="34" max="34" width="16.3516" style="34" customWidth="1"/>
-    <col min="35" max="35" width="16.3516" style="34" customWidth="1"/>
-    <col min="36" max="36" width="16.3516" style="34" customWidth="1"/>
-    <col min="37" max="37" width="16.3516" style="34" customWidth="1"/>
-    <col min="38" max="38" width="16.3516" style="34" customWidth="1"/>
-    <col min="39" max="39" width="16.3516" style="34" customWidth="1"/>
-    <col min="40" max="40" width="16.3516" style="34" customWidth="1"/>
-    <col min="41" max="41" width="16.3516" style="34" customWidth="1"/>
-    <col min="42" max="42" width="16.3516" style="34" customWidth="1"/>
-    <col min="43" max="43" width="16.3516" style="34" customWidth="1"/>
-    <col min="44" max="44" width="16.3516" style="34" customWidth="1"/>
-    <col min="45" max="45" width="16.3516" style="34" customWidth="1"/>
-    <col min="46" max="46" width="16.3516" style="34" customWidth="1"/>
-    <col min="47" max="47" width="16.3516" style="34" customWidth="1"/>
-    <col min="48" max="48" width="16.3516" style="34" customWidth="1"/>
-    <col min="49" max="49" width="16.3516" style="34" customWidth="1"/>
-    <col min="50" max="50" width="16.3516" style="34" customWidth="1"/>
-    <col min="51" max="51" width="16.3516" style="34" customWidth="1"/>
-    <col min="52" max="52" width="16.3516" style="34" customWidth="1"/>
-    <col min="53" max="53" width="16.3516" style="34" customWidth="1"/>
-    <col min="54" max="54" width="16.3516" style="34" customWidth="1"/>
-    <col min="55" max="55" width="16.3516" style="34" customWidth="1"/>
-    <col min="56" max="56" width="16.3516" style="34" customWidth="1"/>
-    <col min="57" max="57" width="16.3516" style="34" customWidth="1"/>
-    <col min="58" max="58" width="16.3516" style="34" customWidth="1"/>
-    <col min="59" max="59" width="16.3516" style="34" customWidth="1"/>
-    <col min="60" max="60" width="16.3516" style="34" customWidth="1"/>
-    <col min="61" max="61" width="16.3516" style="34" customWidth="1"/>
-    <col min="62" max="62" width="16.3516" style="34" customWidth="1"/>
-    <col min="63" max="63" width="16.3516" style="34" customWidth="1"/>
-    <col min="64" max="64" width="16.3516" style="34" customWidth="1"/>
-    <col min="65" max="65" width="16.3516" style="34" customWidth="1"/>
-    <col min="66" max="66" width="16.3516" style="34" customWidth="1"/>
-    <col min="67" max="67" width="16.3516" style="34" customWidth="1"/>
-    <col min="68" max="68" width="16.3516" style="34" customWidth="1"/>
-    <col min="69" max="69" width="16.3516" style="34" customWidth="1"/>
-    <col min="70" max="70" width="16.3516" style="34" customWidth="1"/>
-    <col min="71" max="71" width="16.3516" style="34" customWidth="1"/>
-    <col min="72" max="72" width="16.3516" style="34" customWidth="1"/>
-    <col min="73" max="73" width="16.3516" style="34" customWidth="1"/>
-    <col min="74" max="74" width="16.3516" style="34" customWidth="1"/>
-    <col min="75" max="75" width="16.3516" style="34" customWidth="1"/>
-    <col min="76" max="76" width="16.3516" style="34" customWidth="1"/>
-    <col min="77" max="77" width="16.3516" style="34" customWidth="1"/>
-    <col min="78" max="78" width="16.3516" style="34" customWidth="1"/>
-    <col min="79" max="79" width="16.3516" style="34" customWidth="1"/>
-    <col min="80" max="80" width="16.3516" style="34" customWidth="1"/>
-    <col min="81" max="81" width="16.3516" style="34" customWidth="1"/>
-    <col min="82" max="82" width="16.3516" style="34" customWidth="1"/>
-    <col min="83" max="83" width="16.3516" style="34" customWidth="1"/>
-    <col min="84" max="84" width="16.3516" style="34" customWidth="1"/>
-    <col min="85" max="256" width="16.3516" style="34" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="37" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="37" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="37" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="37" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="37" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="37" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="37" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="37" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="37" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="37" customWidth="1"/>
+    <col min="11" max="11" width="16.3516" style="37" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="37" customWidth="1"/>
+    <col min="13" max="13" width="16.3516" style="37" customWidth="1"/>
+    <col min="14" max="14" width="16.3516" style="37" customWidth="1"/>
+    <col min="15" max="15" width="16.3516" style="37" customWidth="1"/>
+    <col min="16" max="16" width="16.3516" style="37" customWidth="1"/>
+    <col min="17" max="17" width="16.3516" style="37" customWidth="1"/>
+    <col min="18" max="18" width="16.3516" style="37" customWidth="1"/>
+    <col min="19" max="19" width="16.3516" style="37" customWidth="1"/>
+    <col min="20" max="20" width="16.3516" style="37" customWidth="1"/>
+    <col min="21" max="21" width="16.3516" style="37" customWidth="1"/>
+    <col min="22" max="22" width="16.3516" style="37" customWidth="1"/>
+    <col min="23" max="23" width="16.3516" style="37" customWidth="1"/>
+    <col min="24" max="24" width="16.3516" style="37" customWidth="1"/>
+    <col min="25" max="25" width="16.3516" style="37" customWidth="1"/>
+    <col min="26" max="26" width="16.3516" style="37" customWidth="1"/>
+    <col min="27" max="27" width="16.3516" style="37" customWidth="1"/>
+    <col min="28" max="28" width="16.3516" style="37" customWidth="1"/>
+    <col min="29" max="29" width="16.3516" style="37" customWidth="1"/>
+    <col min="30" max="30" width="16.3516" style="37" customWidth="1"/>
+    <col min="31" max="31" width="16.3516" style="37" customWidth="1"/>
+    <col min="32" max="32" width="16.3516" style="37" customWidth="1"/>
+    <col min="33" max="33" width="16.3516" style="37" customWidth="1"/>
+    <col min="34" max="34" width="16.3516" style="37" customWidth="1"/>
+    <col min="35" max="35" width="16.3516" style="37" customWidth="1"/>
+    <col min="36" max="36" width="16.3516" style="37" customWidth="1"/>
+    <col min="37" max="37" width="16.3516" style="37" customWidth="1"/>
+    <col min="38" max="38" width="16.3516" style="37" customWidth="1"/>
+    <col min="39" max="39" width="16.3516" style="37" customWidth="1"/>
+    <col min="40" max="40" width="16.3516" style="37" customWidth="1"/>
+    <col min="41" max="41" width="16.3516" style="37" customWidth="1"/>
+    <col min="42" max="42" width="16.3516" style="37" customWidth="1"/>
+    <col min="43" max="43" width="16.3516" style="37" customWidth="1"/>
+    <col min="44" max="44" width="16.3516" style="37" customWidth="1"/>
+    <col min="45" max="45" width="16.3516" style="37" customWidth="1"/>
+    <col min="46" max="46" width="16.3516" style="37" customWidth="1"/>
+    <col min="47" max="47" width="16.3516" style="37" customWidth="1"/>
+    <col min="48" max="48" width="16.3516" style="37" customWidth="1"/>
+    <col min="49" max="49" width="16.3516" style="37" customWidth="1"/>
+    <col min="50" max="50" width="16.3516" style="37" customWidth="1"/>
+    <col min="51" max="51" width="16.3516" style="37" customWidth="1"/>
+    <col min="52" max="52" width="16.3516" style="37" customWidth="1"/>
+    <col min="53" max="53" width="16.3516" style="37" customWidth="1"/>
+    <col min="54" max="54" width="16.3516" style="37" customWidth="1"/>
+    <col min="55" max="55" width="16.3516" style="37" customWidth="1"/>
+    <col min="56" max="56" width="16.3516" style="37" customWidth="1"/>
+    <col min="57" max="57" width="16.3516" style="37" customWidth="1"/>
+    <col min="58" max="58" width="16.3516" style="37" customWidth="1"/>
+    <col min="59" max="59" width="16.3516" style="37" customWidth="1"/>
+    <col min="60" max="60" width="16.3516" style="37" customWidth="1"/>
+    <col min="61" max="61" width="16.3516" style="37" customWidth="1"/>
+    <col min="62" max="62" width="16.3516" style="37" customWidth="1"/>
+    <col min="63" max="63" width="16.3516" style="37" customWidth="1"/>
+    <col min="64" max="64" width="16.3516" style="37" customWidth="1"/>
+    <col min="65" max="65" width="16.3516" style="37" customWidth="1"/>
+    <col min="66" max="66" width="16.3516" style="37" customWidth="1"/>
+    <col min="67" max="67" width="16.3516" style="37" customWidth="1"/>
+    <col min="68" max="68" width="16.3516" style="37" customWidth="1"/>
+    <col min="69" max="69" width="16.3516" style="37" customWidth="1"/>
+    <col min="70" max="70" width="16.3516" style="37" customWidth="1"/>
+    <col min="71" max="71" width="16.3516" style="37" customWidth="1"/>
+    <col min="72" max="72" width="16.3516" style="37" customWidth="1"/>
+    <col min="73" max="73" width="16.3516" style="37" customWidth="1"/>
+    <col min="74" max="74" width="16.3516" style="37" customWidth="1"/>
+    <col min="75" max="75" width="16.3516" style="37" customWidth="1"/>
+    <col min="76" max="76" width="16.3516" style="37" customWidth="1"/>
+    <col min="77" max="77" width="16.3516" style="37" customWidth="1"/>
+    <col min="78" max="78" width="16.3516" style="37" customWidth="1"/>
+    <col min="79" max="79" width="16.3516" style="37" customWidth="1"/>
+    <col min="80" max="80" width="16.3516" style="37" customWidth="1"/>
+    <col min="81" max="81" width="16.3516" style="37" customWidth="1"/>
+    <col min="82" max="82" width="16.3516" style="37" customWidth="1"/>
+    <col min="83" max="83" width="16.3516" style="37" customWidth="1"/>
+    <col min="84" max="84" width="16.3516" style="37" customWidth="1"/>
+    <col min="85" max="256" width="16.3516" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -25144,91 +25463,91 @@
         <v>20</v>
       </c>
       <c r="C2" t="s" s="21">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s" s="21">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s" s="21">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s" s="21">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G2" t="s" s="21">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s" s="21">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I2" t="s" s="21">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s" s="21">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K2" t="s" s="21">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s" s="21">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M2" t="s" s="21">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N2" t="s" s="21">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="O2" t="s" s="21">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="P2" t="s" s="21">
-        <v>133</v>
-      </c>
-      <c r="Q2" t="s" s="35">
-        <v>134</v>
-      </c>
-      <c r="R2" t="s" s="35">
         <v>135</v>
       </c>
+      <c r="Q2" t="s" s="38">
+        <v>136</v>
+      </c>
+      <c r="R2" t="s" s="38">
+        <v>137</v>
+      </c>
       <c r="S2" t="s" s="21">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="T2" t="s" s="21">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="U2" t="s" s="21">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="V2" t="s" s="21">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="W2" t="s" s="21">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="X2" t="s" s="21">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Y2" t="s" s="21">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="Z2" t="s" s="21">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AA2" t="s" s="21">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AB2" t="s" s="21">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AC2" t="s" s="21">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AD2" t="s" s="21">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AE2" t="s" s="21">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AF2" t="s" s="21">
         <v>27</v>
@@ -25237,10 +25556,10 @@
         <v>63</v>
       </c>
       <c r="AH2" t="s" s="21">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AI2" t="s" s="21">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AJ2" t="s" s="21">
         <v>23</v>
@@ -25249,7 +25568,7 @@
         <v>22</v>
       </c>
       <c r="AL2" t="s" s="21">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AM2" t="s" s="21">
         <v>75</v>
@@ -25270,58 +25589,58 @@
         <v>44</v>
       </c>
       <c r="AS2" t="s" s="21">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AT2" t="s" s="21">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AU2" t="s" s="21">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AV2" t="s" s="21">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AW2" t="s" s="21">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AX2" t="s" s="21">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AY2" t="s" s="21">
         <v>28</v>
       </c>
       <c r="AZ2" t="s" s="21">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="BA2" t="s" s="21">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="BB2" t="s" s="21">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="BC2" t="s" s="21">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="BD2" t="s" s="21">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="BE2" t="s" s="21">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="BF2" t="s" s="21">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="BG2" t="s" s="21">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="BH2" t="s" s="21">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="BI2" t="s" s="21">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="BJ2" t="s" s="21">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="BK2" t="s" s="21">
         <v>56</v>
@@ -25354,31 +25673,31 @@
         <v>73</v>
       </c>
       <c r="BU2" t="s" s="21">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="BV2" t="s" s="21">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="BW2" t="s" s="21">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="BX2" t="s" s="21">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="BY2" t="s" s="21">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="BZ2" t="s" s="21">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="CA2" t="s" s="21">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="CB2" t="s" s="21">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="CC2" t="s" s="21">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="CD2" s="21"/>
       <c r="CE2" s="21"/>
@@ -25386,10 +25705,10 @@
     </row>
     <row r="3" ht="16.55" customHeight="1">
       <c r="A3" t="s" s="22">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s" s="23">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C3" t="s" s="24">
         <v>83</v>
@@ -25428,19 +25747,19 @@
         <v>83</v>
       </c>
       <c r="O3" t="s" s="24">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="P3" t="s" s="24">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Q3" t="s" s="24">
         <v>5</v>
       </c>
       <c r="R3" t="s" s="24">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="S3" t="s" s="24">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="T3" t="s" s="24">
         <v>83</v>
@@ -25458,7 +25777,7 @@
         <v>83</v>
       </c>
       <c r="Y3" t="s" s="24">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="Z3" t="s" s="24">
         <v>83</v>
@@ -25476,7 +25795,7 @@
         <v>90</v>
       </c>
       <c r="AE3" t="s" s="24">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AF3" t="s" s="24">
         <v>83</v>
@@ -25485,46 +25804,46 @@
         <v>5</v>
       </c>
       <c r="AH3" t="s" s="24">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AI3" t="s" s="24">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AJ3" t="s" s="24">
         <v>83</v>
       </c>
       <c r="AK3" t="s" s="24">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AL3" t="s" s="24">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AM3" t="s" s="24">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AN3" t="s" s="24">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AO3" t="s" s="24">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AP3" t="s" s="24">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AQ3" t="s" s="24">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AR3" t="s" s="24">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AS3" t="s" s="24">
         <v>83</v>
       </c>
       <c r="AT3" t="s" s="24">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AU3" t="s" s="24">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AV3" t="s" s="24">
         <v>3</v>
@@ -25539,49 +25858,49 @@
         <v>1</v>
       </c>
       <c r="AZ3" t="s" s="24">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="BA3" t="s" s="24">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="BB3" t="s" s="24">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="BC3" t="s" s="24">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="BD3" t="s" s="24">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="BE3" t="s" s="24">
         <v>0</v>
       </c>
       <c r="BF3" t="s" s="24">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="BG3" t="s" s="24">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="BH3" t="s" s="24">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="BI3" t="s" s="24">
         <v>104</v>
       </c>
       <c r="BJ3" t="s" s="24">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="BK3" t="s" s="24">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="BL3" t="s" s="24">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="BM3" t="s" s="24">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="BN3" t="s" s="24">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="BO3" t="s" s="24">
         <v>109</v>
@@ -25590,7 +25909,7 @@
         <v>1</v>
       </c>
       <c r="BQ3" t="s" s="24">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="BR3" t="s" s="24">
         <v>115</v>
@@ -25599,16 +25918,16 @@
         <v>116</v>
       </c>
       <c r="BT3" t="s" s="24">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="BU3" t="s" s="24">
         <v>5</v>
       </c>
       <c r="BV3" t="s" s="24">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="BW3" t="s" s="24">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="BX3" t="s" s="24">
         <v>83</v>
@@ -25623,7 +25942,7 @@
         <v>83</v>
       </c>
       <c r="CB3" t="s" s="24">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="CC3" t="s" s="24">
         <v>83</v>
@@ -25633,778 +25952,940 @@
       <c r="CF3" s="24"/>
     </row>
     <row r="4" ht="16.35" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="38"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="38"/>
-      <c r="AX4" s="38"/>
-      <c r="AY4" s="38"/>
-      <c r="AZ4" s="38"/>
-      <c r="BA4" s="38"/>
-      <c r="BB4" s="38"/>
-      <c r="BC4" s="38"/>
-      <c r="BD4" s="38"/>
-      <c r="BE4" s="38"/>
-      <c r="BF4" s="38"/>
-      <c r="BG4" s="38"/>
-      <c r="BH4" s="38"/>
-      <c r="BI4" s="38"/>
-      <c r="BJ4" s="38"/>
-      <c r="BK4" s="38"/>
-      <c r="BL4" s="38"/>
-      <c r="BM4" s="38"/>
-      <c r="BN4" s="38"/>
-      <c r="BO4" s="38"/>
-      <c r="BP4" s="38"/>
-      <c r="BQ4" s="38"/>
-      <c r="BR4" s="38"/>
-      <c r="BS4" s="38"/>
-      <c r="BT4" s="38"/>
-      <c r="BU4" s="38"/>
-      <c r="BV4" s="38"/>
-      <c r="BW4" s="38"/>
-      <c r="BX4" s="38"/>
-      <c r="BY4" s="38"/>
-      <c r="BZ4" s="38"/>
-      <c r="CA4" s="38"/>
-      <c r="CB4" s="38"/>
-      <c r="CC4" s="38"/>
-      <c r="CD4" s="38"/>
-      <c r="CE4" s="38"/>
-      <c r="CF4" s="38"/>
+      <c r="A4" t="s" s="25">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>211</v>
+      </c>
+      <c r="C4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="F4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="I4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="L4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="M4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="N4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="O4" t="s" s="27">
+        <v>182</v>
+      </c>
+      <c r="P4" t="s" s="27">
+        <v>183</v>
+      </c>
+      <c r="Q4" t="s" s="27">
+        <v>5</v>
+      </c>
+      <c r="R4" t="s" s="27">
+        <v>183</v>
+      </c>
+      <c r="S4" t="s" s="27">
+        <v>182</v>
+      </c>
+      <c r="T4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="U4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="V4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="W4" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="X4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="Y4" t="s" s="27">
+        <v>184</v>
+      </c>
+      <c r="Z4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AA4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AB4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AC4" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="AD4" t="s" s="27">
+        <v>90</v>
+      </c>
+      <c r="AE4" t="s" s="27">
+        <v>185</v>
+      </c>
+      <c r="AF4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AG4" t="s" s="27">
+        <v>5</v>
+      </c>
+      <c r="AH4" t="s" s="27">
+        <v>183</v>
+      </c>
+      <c r="AI4" t="s" s="27">
+        <v>186</v>
+      </c>
+      <c r="AJ4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AK4" t="s" s="27">
+        <v>182</v>
+      </c>
+      <c r="AL4" t="s" s="27">
+        <v>187</v>
+      </c>
+      <c r="AM4" t="s" s="27">
+        <v>188</v>
+      </c>
+      <c r="AN4" t="s" s="27">
+        <v>189</v>
+      </c>
+      <c r="AO4" t="s" s="27">
+        <v>190</v>
+      </c>
+      <c r="AP4" t="s" s="27">
+        <v>191</v>
+      </c>
+      <c r="AQ4" t="s" s="27">
+        <v>192</v>
+      </c>
+      <c r="AR4" t="s" s="27">
+        <v>193</v>
+      </c>
+      <c r="AS4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="AT4" t="s" s="27">
+        <v>194</v>
+      </c>
+      <c r="AU4" t="s" s="27">
+        <v>195</v>
+      </c>
+      <c r="AV4" t="s" s="27">
+        <v>3</v>
+      </c>
+      <c r="AW4" t="s" s="27">
+        <v>2</v>
+      </c>
+      <c r="AX4" t="s" s="27">
+        <v>2</v>
+      </c>
+      <c r="AY4" t="s" s="27">
+        <v>1</v>
+      </c>
+      <c r="AZ4" t="s" s="27">
+        <v>196</v>
+      </c>
+      <c r="BA4" t="s" s="27">
+        <v>197</v>
+      </c>
+      <c r="BB4" t="s" s="27">
+        <v>198</v>
+      </c>
+      <c r="BC4" t="s" s="27">
+        <v>199</v>
+      </c>
+      <c r="BD4" t="s" s="27">
+        <v>200</v>
+      </c>
+      <c r="BE4" t="s" s="27">
+        <v>0</v>
+      </c>
+      <c r="BF4" t="s" s="27">
+        <v>201</v>
+      </c>
+      <c r="BG4" t="s" s="27">
+        <v>202</v>
+      </c>
+      <c r="BH4" t="s" s="27">
+        <v>203</v>
+      </c>
+      <c r="BI4" t="s" s="27">
+        <v>104</v>
+      </c>
+      <c r="BJ4" t="s" s="27">
+        <v>204</v>
+      </c>
+      <c r="BK4" t="s" s="27">
+        <v>205</v>
+      </c>
+      <c r="BL4" t="s" s="27">
+        <v>206</v>
+      </c>
+      <c r="BM4" t="s" s="27">
+        <v>207</v>
+      </c>
+      <c r="BN4" t="s" s="27">
+        <v>208</v>
+      </c>
+      <c r="BO4" t="s" s="27">
+        <v>109</v>
+      </c>
+      <c r="BP4" t="s" s="27">
+        <v>1</v>
+      </c>
+      <c r="BQ4" t="s" s="27">
+        <v>209</v>
+      </c>
+      <c r="BR4" t="s" s="27">
+        <v>115</v>
+      </c>
+      <c r="BS4" t="s" s="27">
+        <v>116</v>
+      </c>
+      <c r="BT4" t="s" s="27">
+        <v>194</v>
+      </c>
+      <c r="BU4" t="s" s="27">
+        <v>5</v>
+      </c>
+      <c r="BV4" t="s" s="27">
+        <v>195</v>
+      </c>
+      <c r="BW4" t="s" s="27">
+        <v>194</v>
+      </c>
+      <c r="BX4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="BY4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="BZ4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="CA4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="CB4" t="s" s="27">
+        <v>210</v>
+      </c>
+      <c r="CC4" t="s" s="27">
+        <v>83</v>
+      </c>
+      <c r="CD4" s="27"/>
+      <c r="CE4" s="27"/>
+      <c r="CF4" s="27"/>
     </row>
     <row r="5" ht="16.35" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
-      <c r="AI5" s="38"/>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="38"/>
-      <c r="AO5" s="38"/>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="38"/>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
-      <c r="AV5" s="38"/>
-      <c r="AW5" s="38"/>
-      <c r="AX5" s="38"/>
-      <c r="AY5" s="38"/>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="38"/>
-      <c r="BB5" s="38"/>
-      <c r="BC5" s="38"/>
-      <c r="BD5" s="38"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="38"/>
-      <c r="BG5" s="38"/>
-      <c r="BH5" s="38"/>
-      <c r="BI5" s="38"/>
-      <c r="BJ5" s="38"/>
-      <c r="BK5" s="38"/>
-      <c r="BL5" s="38"/>
-      <c r="BM5" s="38"/>
-      <c r="BN5" s="38"/>
-      <c r="BO5" s="38"/>
-      <c r="BP5" s="38"/>
-      <c r="BQ5" s="38"/>
-      <c r="BR5" s="38"/>
-      <c r="BS5" s="38"/>
-      <c r="BT5" s="38"/>
-      <c r="BU5" s="38"/>
-      <c r="BV5" s="38"/>
-      <c r="BW5" s="38"/>
-      <c r="BX5" s="38"/>
-      <c r="BY5" s="38"/>
-      <c r="BZ5" s="38"/>
-      <c r="CA5" s="38"/>
-      <c r="CB5" s="38"/>
-      <c r="CC5" s="38"/>
-      <c r="CD5" s="38"/>
-      <c r="CE5" s="38"/>
-      <c r="CF5" s="38"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="41"/>
+      <c r="AF5" s="41"/>
+      <c r="AG5" s="41"/>
+      <c r="AH5" s="41"/>
+      <c r="AI5" s="41"/>
+      <c r="AJ5" s="41"/>
+      <c r="AK5" s="41"/>
+      <c r="AL5" s="41"/>
+      <c r="AM5" s="41"/>
+      <c r="AN5" s="41"/>
+      <c r="AO5" s="41"/>
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="41"/>
+      <c r="AR5" s="41"/>
+      <c r="AS5" s="41"/>
+      <c r="AT5" s="41"/>
+      <c r="AU5" s="41"/>
+      <c r="AV5" s="41"/>
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="41"/>
+      <c r="AZ5" s="41"/>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="41"/>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="41"/>
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="41"/>
+      <c r="BN5" s="41"/>
+      <c r="BO5" s="41"/>
+      <c r="BP5" s="41"/>
+      <c r="BQ5" s="41"/>
+      <c r="BR5" s="41"/>
+      <c r="BS5" s="41"/>
+      <c r="BT5" s="41"/>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="41"/>
+      <c r="BW5" s="41"/>
+      <c r="BX5" s="41"/>
+      <c r="BY5" s="41"/>
+      <c r="BZ5" s="41"/>
+      <c r="CA5" s="41"/>
+      <c r="CB5" s="41"/>
+      <c r="CC5" s="41"/>
+      <c r="CD5" s="41"/>
+      <c r="CE5" s="41"/>
+      <c r="CF5" s="41"/>
     </row>
     <row r="6" ht="16.35" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="38"/>
-      <c r="AL6" s="38"/>
-      <c r="AM6" s="38"/>
-      <c r="AN6" s="38"/>
-      <c r="AO6" s="38"/>
-      <c r="AP6" s="38"/>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="38"/>
-      <c r="AS6" s="38"/>
-      <c r="AT6" s="38"/>
-      <c r="AU6" s="38"/>
-      <c r="AV6" s="38"/>
-      <c r="AW6" s="38"/>
-      <c r="AX6" s="38"/>
-      <c r="AY6" s="38"/>
-      <c r="AZ6" s="38"/>
-      <c r="BA6" s="38"/>
-      <c r="BB6" s="38"/>
-      <c r="BC6" s="38"/>
-      <c r="BD6" s="38"/>
-      <c r="BE6" s="38"/>
-      <c r="BF6" s="38"/>
-      <c r="BG6" s="38"/>
-      <c r="BH6" s="38"/>
-      <c r="BI6" s="38"/>
-      <c r="BJ6" s="38"/>
-      <c r="BK6" s="38"/>
-      <c r="BL6" s="38"/>
-      <c r="BM6" s="38"/>
-      <c r="BN6" s="38"/>
-      <c r="BO6" s="38"/>
-      <c r="BP6" s="38"/>
-      <c r="BQ6" s="38"/>
-      <c r="BR6" s="38"/>
-      <c r="BS6" s="38"/>
-      <c r="BT6" s="38"/>
-      <c r="BU6" s="38"/>
-      <c r="BV6" s="38"/>
-      <c r="BW6" s="38"/>
-      <c r="BX6" s="38"/>
-      <c r="BY6" s="38"/>
-      <c r="BZ6" s="38"/>
-      <c r="CA6" s="38"/>
-      <c r="CB6" s="38"/>
-      <c r="CC6" s="38"/>
-      <c r="CD6" s="38"/>
-      <c r="CE6" s="38"/>
-      <c r="CF6" s="38"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
+      <c r="AE6" s="41"/>
+      <c r="AF6" s="41"/>
+      <c r="AG6" s="41"/>
+      <c r="AH6" s="41"/>
+      <c r="AI6" s="41"/>
+      <c r="AJ6" s="41"/>
+      <c r="AK6" s="41"/>
+      <c r="AL6" s="41"/>
+      <c r="AM6" s="41"/>
+      <c r="AN6" s="41"/>
+      <c r="AO6" s="41"/>
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="41"/>
+      <c r="AR6" s="41"/>
+      <c r="AS6" s="41"/>
+      <c r="AT6" s="41"/>
+      <c r="AU6" s="41"/>
+      <c r="AV6" s="41"/>
+      <c r="AW6" s="41"/>
+      <c r="AX6" s="41"/>
+      <c r="AY6" s="41"/>
+      <c r="AZ6" s="41"/>
+      <c r="BA6" s="41"/>
+      <c r="BB6" s="41"/>
+      <c r="BC6" s="41"/>
+      <c r="BD6" s="41"/>
+      <c r="BE6" s="41"/>
+      <c r="BF6" s="41"/>
+      <c r="BG6" s="41"/>
+      <c r="BH6" s="41"/>
+      <c r="BI6" s="41"/>
+      <c r="BJ6" s="41"/>
+      <c r="BK6" s="41"/>
+      <c r="BL6" s="41"/>
+      <c r="BM6" s="41"/>
+      <c r="BN6" s="41"/>
+      <c r="BO6" s="41"/>
+      <c r="BP6" s="41"/>
+      <c r="BQ6" s="41"/>
+      <c r="BR6" s="41"/>
+      <c r="BS6" s="41"/>
+      <c r="BT6" s="41"/>
+      <c r="BU6" s="41"/>
+      <c r="BV6" s="41"/>
+      <c r="BW6" s="41"/>
+      <c r="BX6" s="41"/>
+      <c r="BY6" s="41"/>
+      <c r="BZ6" s="41"/>
+      <c r="CA6" s="41"/>
+      <c r="CB6" s="41"/>
+      <c r="CC6" s="41"/>
+      <c r="CD6" s="41"/>
+      <c r="CE6" s="41"/>
+      <c r="CF6" s="41"/>
     </row>
     <row r="7" ht="16.35" customHeight="1">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
-      <c r="AC7" s="38"/>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="38"/>
-      <c r="AF7" s="38"/>
-      <c r="AG7" s="38"/>
-      <c r="AH7" s="38"/>
-      <c r="AI7" s="38"/>
-      <c r="AJ7" s="38"/>
-      <c r="AK7" s="38"/>
-      <c r="AL7" s="38"/>
-      <c r="AM7" s="38"/>
-      <c r="AN7" s="38"/>
-      <c r="AO7" s="38"/>
-      <c r="AP7" s="38"/>
-      <c r="AQ7" s="38"/>
-      <c r="AR7" s="38"/>
-      <c r="AS7" s="38"/>
-      <c r="AT7" s="38"/>
-      <c r="AU7" s="38"/>
-      <c r="AV7" s="38"/>
-      <c r="AW7" s="38"/>
-      <c r="AX7" s="38"/>
-      <c r="AY7" s="38"/>
-      <c r="AZ7" s="38"/>
-      <c r="BA7" s="38"/>
-      <c r="BB7" s="38"/>
-      <c r="BC7" s="38"/>
-      <c r="BD7" s="38"/>
-      <c r="BE7" s="38"/>
-      <c r="BF7" s="38"/>
-      <c r="BG7" s="38"/>
-      <c r="BH7" s="38"/>
-      <c r="BI7" s="38"/>
-      <c r="BJ7" s="38"/>
-      <c r="BK7" s="38"/>
-      <c r="BL7" s="38"/>
-      <c r="BM7" s="38"/>
-      <c r="BN7" s="38"/>
-      <c r="BO7" s="38"/>
-      <c r="BP7" s="38"/>
-      <c r="BQ7" s="38"/>
-      <c r="BR7" s="38"/>
-      <c r="BS7" s="38"/>
-      <c r="BT7" s="38"/>
-      <c r="BU7" s="38"/>
-      <c r="BV7" s="38"/>
-      <c r="BW7" s="38"/>
-      <c r="BX7" s="38"/>
-      <c r="BY7" s="38"/>
-      <c r="BZ7" s="38"/>
-      <c r="CA7" s="38"/>
-      <c r="CB7" s="38"/>
-      <c r="CC7" s="38"/>
-      <c r="CD7" s="38"/>
-      <c r="CE7" s="38"/>
-      <c r="CF7" s="38"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
+      <c r="AH7" s="41"/>
+      <c r="AI7" s="41"/>
+      <c r="AJ7" s="41"/>
+      <c r="AK7" s="41"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="41"/>
+      <c r="AQ7" s="41"/>
+      <c r="AR7" s="41"/>
+      <c r="AS7" s="41"/>
+      <c r="AT7" s="41"/>
+      <c r="AU7" s="41"/>
+      <c r="AV7" s="41"/>
+      <c r="AW7" s="41"/>
+      <c r="AX7" s="41"/>
+      <c r="AY7" s="41"/>
+      <c r="AZ7" s="41"/>
+      <c r="BA7" s="41"/>
+      <c r="BB7" s="41"/>
+      <c r="BC7" s="41"/>
+      <c r="BD7" s="41"/>
+      <c r="BE7" s="41"/>
+      <c r="BF7" s="41"/>
+      <c r="BG7" s="41"/>
+      <c r="BH7" s="41"/>
+      <c r="BI7" s="41"/>
+      <c r="BJ7" s="41"/>
+      <c r="BK7" s="41"/>
+      <c r="BL7" s="41"/>
+      <c r="BM7" s="41"/>
+      <c r="BN7" s="41"/>
+      <c r="BO7" s="41"/>
+      <c r="BP7" s="41"/>
+      <c r="BQ7" s="41"/>
+      <c r="BR7" s="41"/>
+      <c r="BS7" s="41"/>
+      <c r="BT7" s="41"/>
+      <c r="BU7" s="41"/>
+      <c r="BV7" s="41"/>
+      <c r="BW7" s="41"/>
+      <c r="BX7" s="41"/>
+      <c r="BY7" s="41"/>
+      <c r="BZ7" s="41"/>
+      <c r="CA7" s="41"/>
+      <c r="CB7" s="41"/>
+      <c r="CC7" s="41"/>
+      <c r="CD7" s="41"/>
+      <c r="CE7" s="41"/>
+      <c r="CF7" s="41"/>
     </row>
     <row r="8" ht="16.35" customHeight="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38"/>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="38"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
-      <c r="AI8" s="38"/>
-      <c r="AJ8" s="38"/>
-      <c r="AK8" s="38"/>
-      <c r="AL8" s="38"/>
-      <c r="AM8" s="38"/>
-      <c r="AN8" s="38"/>
-      <c r="AO8" s="38"/>
-      <c r="AP8" s="38"/>
-      <c r="AQ8" s="38"/>
-      <c r="AR8" s="38"/>
-      <c r="AS8" s="38"/>
-      <c r="AT8" s="38"/>
-      <c r="AU8" s="38"/>
-      <c r="AV8" s="38"/>
-      <c r="AW8" s="38"/>
-      <c r="AX8" s="38"/>
-      <c r="AY8" s="38"/>
-      <c r="AZ8" s="38"/>
-      <c r="BA8" s="38"/>
-      <c r="BB8" s="38"/>
-      <c r="BC8" s="38"/>
-      <c r="BD8" s="38"/>
-      <c r="BE8" s="38"/>
-      <c r="BF8" s="38"/>
-      <c r="BG8" s="38"/>
-      <c r="BH8" s="38"/>
-      <c r="BI8" s="38"/>
-      <c r="BJ8" s="38"/>
-      <c r="BK8" s="38"/>
-      <c r="BL8" s="38"/>
-      <c r="BM8" s="38"/>
-      <c r="BN8" s="38"/>
-      <c r="BO8" s="38"/>
-      <c r="BP8" s="38"/>
-      <c r="BQ8" s="38"/>
-      <c r="BR8" s="38"/>
-      <c r="BS8" s="38"/>
-      <c r="BT8" s="38"/>
-      <c r="BU8" s="38"/>
-      <c r="BV8" s="38"/>
-      <c r="BW8" s="38"/>
-      <c r="BX8" s="38"/>
-      <c r="BY8" s="38"/>
-      <c r="BZ8" s="38"/>
-      <c r="CA8" s="38"/>
-      <c r="CB8" s="38"/>
-      <c r="CC8" s="38"/>
-      <c r="CD8" s="38"/>
-      <c r="CE8" s="38"/>
-      <c r="CF8" s="38"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="41"/>
+      <c r="AF8" s="41"/>
+      <c r="AG8" s="41"/>
+      <c r="AH8" s="41"/>
+      <c r="AI8" s="41"/>
+      <c r="AJ8" s="41"/>
+      <c r="AK8" s="41"/>
+      <c r="AL8" s="41"/>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="41"/>
+      <c r="AO8" s="41"/>
+      <c r="AP8" s="41"/>
+      <c r="AQ8" s="41"/>
+      <c r="AR8" s="41"/>
+      <c r="AS8" s="41"/>
+      <c r="AT8" s="41"/>
+      <c r="AU8" s="41"/>
+      <c r="AV8" s="41"/>
+      <c r="AW8" s="41"/>
+      <c r="AX8" s="41"/>
+      <c r="AY8" s="41"/>
+      <c r="AZ8" s="41"/>
+      <c r="BA8" s="41"/>
+      <c r="BB8" s="41"/>
+      <c r="BC8" s="41"/>
+      <c r="BD8" s="41"/>
+      <c r="BE8" s="41"/>
+      <c r="BF8" s="41"/>
+      <c r="BG8" s="41"/>
+      <c r="BH8" s="41"/>
+      <c r="BI8" s="41"/>
+      <c r="BJ8" s="41"/>
+      <c r="BK8" s="41"/>
+      <c r="BL8" s="41"/>
+      <c r="BM8" s="41"/>
+      <c r="BN8" s="41"/>
+      <c r="BO8" s="41"/>
+      <c r="BP8" s="41"/>
+      <c r="BQ8" s="41"/>
+      <c r="BR8" s="41"/>
+      <c r="BS8" s="41"/>
+      <c r="BT8" s="41"/>
+      <c r="BU8" s="41"/>
+      <c r="BV8" s="41"/>
+      <c r="BW8" s="41"/>
+      <c r="BX8" s="41"/>
+      <c r="BY8" s="41"/>
+      <c r="BZ8" s="41"/>
+      <c r="CA8" s="41"/>
+      <c r="CB8" s="41"/>
+      <c r="CC8" s="41"/>
+      <c r="CD8" s="41"/>
+      <c r="CE8" s="41"/>
+      <c r="CF8" s="41"/>
     </row>
     <row r="9" ht="16.35" customHeight="1">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="38"/>
-      <c r="AJ9" s="38"/>
-      <c r="AK9" s="38"/>
-      <c r="AL9" s="38"/>
-      <c r="AM9" s="38"/>
-      <c r="AN9" s="38"/>
-      <c r="AO9" s="38"/>
-      <c r="AP9" s="38"/>
-      <c r="AQ9" s="38"/>
-      <c r="AR9" s="38"/>
-      <c r="AS9" s="38"/>
-      <c r="AT9" s="38"/>
-      <c r="AU9" s="38"/>
-      <c r="AV9" s="38"/>
-      <c r="AW9" s="38"/>
-      <c r="AX9" s="38"/>
-      <c r="AY9" s="38"/>
-      <c r="AZ9" s="38"/>
-      <c r="BA9" s="38"/>
-      <c r="BB9" s="38"/>
-      <c r="BC9" s="38"/>
-      <c r="BD9" s="38"/>
-      <c r="BE9" s="38"/>
-      <c r="BF9" s="38"/>
-      <c r="BG9" s="38"/>
-      <c r="BH9" s="38"/>
-      <c r="BI9" s="38"/>
-      <c r="BJ9" s="38"/>
-      <c r="BK9" s="38"/>
-      <c r="BL9" s="38"/>
-      <c r="BM9" s="38"/>
-      <c r="BN9" s="38"/>
-      <c r="BO9" s="38"/>
-      <c r="BP9" s="38"/>
-      <c r="BQ9" s="38"/>
-      <c r="BR9" s="38"/>
-      <c r="BS9" s="38"/>
-      <c r="BT9" s="38"/>
-      <c r="BU9" s="38"/>
-      <c r="BV9" s="38"/>
-      <c r="BW9" s="38"/>
-      <c r="BX9" s="38"/>
-      <c r="BY9" s="38"/>
-      <c r="BZ9" s="38"/>
-      <c r="CA9" s="38"/>
-      <c r="CB9" s="38"/>
-      <c r="CC9" s="38"/>
-      <c r="CD9" s="38"/>
-      <c r="CE9" s="38"/>
-      <c r="CF9" s="38"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="41"/>
+      <c r="AD9" s="41"/>
+      <c r="AE9" s="41"/>
+      <c r="AF9" s="41"/>
+      <c r="AG9" s="41"/>
+      <c r="AH9" s="41"/>
+      <c r="AI9" s="41"/>
+      <c r="AJ9" s="41"/>
+      <c r="AK9" s="41"/>
+      <c r="AL9" s="41"/>
+      <c r="AM9" s="41"/>
+      <c r="AN9" s="41"/>
+      <c r="AO9" s="41"/>
+      <c r="AP9" s="41"/>
+      <c r="AQ9" s="41"/>
+      <c r="AR9" s="41"/>
+      <c r="AS9" s="41"/>
+      <c r="AT9" s="41"/>
+      <c r="AU9" s="41"/>
+      <c r="AV9" s="41"/>
+      <c r="AW9" s="41"/>
+      <c r="AX9" s="41"/>
+      <c r="AY9" s="41"/>
+      <c r="AZ9" s="41"/>
+      <c r="BA9" s="41"/>
+      <c r="BB9" s="41"/>
+      <c r="BC9" s="41"/>
+      <c r="BD9" s="41"/>
+      <c r="BE9" s="41"/>
+      <c r="BF9" s="41"/>
+      <c r="BG9" s="41"/>
+      <c r="BH9" s="41"/>
+      <c r="BI9" s="41"/>
+      <c r="BJ9" s="41"/>
+      <c r="BK9" s="41"/>
+      <c r="BL9" s="41"/>
+      <c r="BM9" s="41"/>
+      <c r="BN9" s="41"/>
+      <c r="BO9" s="41"/>
+      <c r="BP9" s="41"/>
+      <c r="BQ9" s="41"/>
+      <c r="BR9" s="41"/>
+      <c r="BS9" s="41"/>
+      <c r="BT9" s="41"/>
+      <c r="BU9" s="41"/>
+      <c r="BV9" s="41"/>
+      <c r="BW9" s="41"/>
+      <c r="BX9" s="41"/>
+      <c r="BY9" s="41"/>
+      <c r="BZ9" s="41"/>
+      <c r="CA9" s="41"/>
+      <c r="CB9" s="41"/>
+      <c r="CC9" s="41"/>
+      <c r="CD9" s="41"/>
+      <c r="CE9" s="41"/>
+      <c r="CF9" s="41"/>
     </row>
     <row r="10" ht="16.35" customHeight="1">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="38"/>
-      <c r="AJ10" s="38"/>
-      <c r="AK10" s="38"/>
-      <c r="AL10" s="38"/>
-      <c r="AM10" s="38"/>
-      <c r="AN10" s="38"/>
-      <c r="AO10" s="38"/>
-      <c r="AP10" s="38"/>
-      <c r="AQ10" s="38"/>
-      <c r="AR10" s="38"/>
-      <c r="AS10" s="38"/>
-      <c r="AT10" s="38"/>
-      <c r="AU10" s="38"/>
-      <c r="AV10" s="38"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="38"/>
-      <c r="BA10" s="38"/>
-      <c r="BB10" s="38"/>
-      <c r="BC10" s="38"/>
-      <c r="BD10" s="38"/>
-      <c r="BE10" s="38"/>
-      <c r="BF10" s="38"/>
-      <c r="BG10" s="38"/>
-      <c r="BH10" s="38"/>
-      <c r="BI10" s="38"/>
-      <c r="BJ10" s="38"/>
-      <c r="BK10" s="38"/>
-      <c r="BL10" s="38"/>
-      <c r="BM10" s="38"/>
-      <c r="BN10" s="38"/>
-      <c r="BO10" s="38"/>
-      <c r="BP10" s="38"/>
-      <c r="BQ10" s="38"/>
-      <c r="BR10" s="38"/>
-      <c r="BS10" s="38"/>
-      <c r="BT10" s="38"/>
-      <c r="BU10" s="38"/>
-      <c r="BV10" s="38"/>
-      <c r="BW10" s="38"/>
-      <c r="BX10" s="38"/>
-      <c r="BY10" s="38"/>
-      <c r="BZ10" s="38"/>
-      <c r="CA10" s="38"/>
-      <c r="CB10" s="38"/>
-      <c r="CC10" s="38"/>
-      <c r="CD10" s="38"/>
-      <c r="CE10" s="38"/>
-      <c r="CF10" s="38"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="41"/>
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="41"/>
+      <c r="AH10" s="41"/>
+      <c r="AI10" s="41"/>
+      <c r="AJ10" s="41"/>
+      <c r="AK10" s="41"/>
+      <c r="AL10" s="41"/>
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="41"/>
+      <c r="AQ10" s="41"/>
+      <c r="AR10" s="41"/>
+      <c r="AS10" s="41"/>
+      <c r="AT10" s="41"/>
+      <c r="AU10" s="41"/>
+      <c r="AV10" s="41"/>
+      <c r="AW10" s="41"/>
+      <c r="AX10" s="41"/>
+      <c r="AY10" s="41"/>
+      <c r="AZ10" s="41"/>
+      <c r="BA10" s="41"/>
+      <c r="BB10" s="41"/>
+      <c r="BC10" s="41"/>
+      <c r="BD10" s="41"/>
+      <c r="BE10" s="41"/>
+      <c r="BF10" s="41"/>
+      <c r="BG10" s="41"/>
+      <c r="BH10" s="41"/>
+      <c r="BI10" s="41"/>
+      <c r="BJ10" s="41"/>
+      <c r="BK10" s="41"/>
+      <c r="BL10" s="41"/>
+      <c r="BM10" s="41"/>
+      <c r="BN10" s="41"/>
+      <c r="BO10" s="41"/>
+      <c r="BP10" s="41"/>
+      <c r="BQ10" s="41"/>
+      <c r="BR10" s="41"/>
+      <c r="BS10" s="41"/>
+      <c r="BT10" s="41"/>
+      <c r="BU10" s="41"/>
+      <c r="BV10" s="41"/>
+      <c r="BW10" s="41"/>
+      <c r="BX10" s="41"/>
+      <c r="BY10" s="41"/>
+      <c r="BZ10" s="41"/>
+      <c r="CA10" s="41"/>
+      <c r="CB10" s="41"/>
+      <c r="CC10" s="41"/>
+      <c r="CD10" s="41"/>
+      <c r="CE10" s="41"/>
+      <c r="CF10" s="41"/>
     </row>
     <row r="11" ht="16.35" customHeight="1">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="38"/>
-      <c r="AK11" s="38"/>
-      <c r="AL11" s="38"/>
-      <c r="AM11" s="38"/>
-      <c r="AN11" s="38"/>
-      <c r="AO11" s="38"/>
-      <c r="AP11" s="38"/>
-      <c r="AQ11" s="38"/>
-      <c r="AR11" s="38"/>
-      <c r="AS11" s="38"/>
-      <c r="AT11" s="38"/>
-      <c r="AU11" s="38"/>
-      <c r="AV11" s="38"/>
-      <c r="AW11" s="38"/>
-      <c r="AX11" s="38"/>
-      <c r="AY11" s="38"/>
-      <c r="AZ11" s="38"/>
-      <c r="BA11" s="38"/>
-      <c r="BB11" s="38"/>
-      <c r="BC11" s="38"/>
-      <c r="BD11" s="38"/>
-      <c r="BE11" s="38"/>
-      <c r="BF11" s="38"/>
-      <c r="BG11" s="38"/>
-      <c r="BH11" s="38"/>
-      <c r="BI11" s="38"/>
-      <c r="BJ11" s="38"/>
-      <c r="BK11" s="38"/>
-      <c r="BL11" s="38"/>
-      <c r="BM11" s="38"/>
-      <c r="BN11" s="38"/>
-      <c r="BO11" s="38"/>
-      <c r="BP11" s="38"/>
-      <c r="BQ11" s="38"/>
-      <c r="BR11" s="38"/>
-      <c r="BS11" s="38"/>
-      <c r="BT11" s="38"/>
-      <c r="BU11" s="38"/>
-      <c r="BV11" s="38"/>
-      <c r="BW11" s="38"/>
-      <c r="BX11" s="38"/>
-      <c r="BY11" s="38"/>
-      <c r="BZ11" s="38"/>
-      <c r="CA11" s="38"/>
-      <c r="CB11" s="38"/>
-      <c r="CC11" s="38"/>
-      <c r="CD11" s="38"/>
-      <c r="CE11" s="38"/>
-      <c r="CF11" s="38"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
+      <c r="AD11" s="41"/>
+      <c r="AE11" s="41"/>
+      <c r="AF11" s="41"/>
+      <c r="AG11" s="41"/>
+      <c r="AH11" s="41"/>
+      <c r="AI11" s="41"/>
+      <c r="AJ11" s="41"/>
+      <c r="AK11" s="41"/>
+      <c r="AL11" s="41"/>
+      <c r="AM11" s="41"/>
+      <c r="AN11" s="41"/>
+      <c r="AO11" s="41"/>
+      <c r="AP11" s="41"/>
+      <c r="AQ11" s="41"/>
+      <c r="AR11" s="41"/>
+      <c r="AS11" s="41"/>
+      <c r="AT11" s="41"/>
+      <c r="AU11" s="41"/>
+      <c r="AV11" s="41"/>
+      <c r="AW11" s="41"/>
+      <c r="AX11" s="41"/>
+      <c r="AY11" s="41"/>
+      <c r="AZ11" s="41"/>
+      <c r="BA11" s="41"/>
+      <c r="BB11" s="41"/>
+      <c r="BC11" s="41"/>
+      <c r="BD11" s="41"/>
+      <c r="BE11" s="41"/>
+      <c r="BF11" s="41"/>
+      <c r="BG11" s="41"/>
+      <c r="BH11" s="41"/>
+      <c r="BI11" s="41"/>
+      <c r="BJ11" s="41"/>
+      <c r="BK11" s="41"/>
+      <c r="BL11" s="41"/>
+      <c r="BM11" s="41"/>
+      <c r="BN11" s="41"/>
+      <c r="BO11" s="41"/>
+      <c r="BP11" s="41"/>
+      <c r="BQ11" s="41"/>
+      <c r="BR11" s="41"/>
+      <c r="BS11" s="41"/>
+      <c r="BT11" s="41"/>
+      <c r="BU11" s="41"/>
+      <c r="BV11" s="41"/>
+      <c r="BW11" s="41"/>
+      <c r="BX11" s="41"/>
+      <c r="BY11" s="41"/>
+      <c r="BZ11" s="41"/>
+      <c r="CA11" s="41"/>
+      <c r="CB11" s="41"/>
+      <c r="CC11" s="41"/>
+      <c r="CD11" s="41"/>
+      <c r="CE11" s="41"/>
+      <c r="CF11" s="41"/>
     </row>
     <row r="12" ht="15.9" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="29"/>
-      <c r="AD12" s="29"/>
-      <c r="AE12" s="29"/>
-      <c r="AF12" s="29"/>
-      <c r="AG12" s="29"/>
-      <c r="AH12" s="29"/>
-      <c r="AI12" s="29"/>
-      <c r="AJ12" s="29"/>
-      <c r="AK12" s="29"/>
-      <c r="AL12" s="29"/>
-      <c r="AM12" s="29"/>
-      <c r="AN12" s="29"/>
-      <c r="AO12" s="29"/>
-      <c r="AP12" s="29"/>
-      <c r="AQ12" s="29"/>
-      <c r="AR12" s="29"/>
-      <c r="AS12" s="29"/>
-      <c r="AT12" s="29"/>
-      <c r="AU12" s="29"/>
-      <c r="AV12" s="29"/>
-      <c r="AW12" s="29"/>
-      <c r="AX12" s="29"/>
-      <c r="AY12" s="29"/>
-      <c r="AZ12" s="29"/>
-      <c r="BA12" s="29"/>
-      <c r="BB12" s="29"/>
-      <c r="BC12" s="29"/>
-      <c r="BD12" s="29"/>
-      <c r="BE12" s="29"/>
-      <c r="BF12" s="29"/>
-      <c r="BG12" s="29"/>
-      <c r="BH12" s="29"/>
-      <c r="BI12" s="29"/>
-      <c r="BJ12" s="29"/>
-      <c r="BK12" s="29"/>
-      <c r="BL12" s="29"/>
-      <c r="BM12" s="29"/>
-      <c r="BN12" s="29"/>
-      <c r="BO12" s="29"/>
-      <c r="BP12" s="29"/>
-      <c r="BQ12" s="29"/>
-      <c r="BR12" s="29"/>
-      <c r="BS12" s="29"/>
-      <c r="BT12" s="29"/>
-      <c r="BU12" s="29"/>
-      <c r="BV12" s="29"/>
-      <c r="BW12" s="29"/>
-      <c r="BX12" s="29"/>
-      <c r="BY12" s="29"/>
-      <c r="BZ12" s="29"/>
-      <c r="CA12" s="29"/>
-      <c r="CB12" s="29"/>
-      <c r="CC12" s="29"/>
-      <c r="CD12" s="29"/>
-      <c r="CE12" s="29"/>
-      <c r="CF12" s="30"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
+      <c r="AI12" s="32"/>
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="32"/>
+      <c r="AL12" s="32"/>
+      <c r="AM12" s="32"/>
+      <c r="AN12" s="32"/>
+      <c r="AO12" s="32"/>
+      <c r="AP12" s="32"/>
+      <c r="AQ12" s="32"/>
+      <c r="AR12" s="32"/>
+      <c r="AS12" s="32"/>
+      <c r="AT12" s="32"/>
+      <c r="AU12" s="32"/>
+      <c r="AV12" s="32"/>
+      <c r="AW12" s="32"/>
+      <c r="AX12" s="32"/>
+      <c r="AY12" s="32"/>
+      <c r="AZ12" s="32"/>
+      <c r="BA12" s="32"/>
+      <c r="BB12" s="32"/>
+      <c r="BC12" s="32"/>
+      <c r="BD12" s="32"/>
+      <c r="BE12" s="32"/>
+      <c r="BF12" s="32"/>
+      <c r="BG12" s="32"/>
+      <c r="BH12" s="32"/>
+      <c r="BI12" s="32"/>
+      <c r="BJ12" s="32"/>
+      <c r="BK12" s="32"/>
+      <c r="BL12" s="32"/>
+      <c r="BM12" s="32"/>
+      <c r="BN12" s="32"/>
+      <c r="BO12" s="32"/>
+      <c r="BP12" s="32"/>
+      <c r="BQ12" s="32"/>
+      <c r="BR12" s="32"/>
+      <c r="BS12" s="32"/>
+      <c r="BT12" s="32"/>
+      <c r="BU12" s="32"/>
+      <c r="BV12" s="32"/>
+      <c r="BW12" s="32"/>
+      <c r="BX12" s="32"/>
+      <c r="BY12" s="32"/>
+      <c r="BZ12" s="32"/>
+      <c r="CA12" s="32"/>
+      <c r="CB12" s="32"/>
+      <c r="CC12" s="32"/>
+      <c r="CD12" s="32"/>
+      <c r="CE12" s="32"/>
+      <c r="CF12" s="33"/>
     </row>
     <row r="13" ht="15.9" customHeight="1">
       <c r="A13" s="6"/>
@@ -35786,13 +36267,14 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="BO3" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="BO4" r:id="rId2" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -35807,240 +36289,240 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="39" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="39" customWidth="1"/>
-    <col min="3" max="3" width="18.6719" style="39" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="39" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="39" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="39" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="39" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="39" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="39" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="39" customWidth="1"/>
-    <col min="11" max="11" width="16.3516" style="39" customWidth="1"/>
-    <col min="12" max="12" width="16.3516" style="39" customWidth="1"/>
-    <col min="13" max="13" width="16.3516" style="39" customWidth="1"/>
-    <col min="14" max="256" width="16.3516" style="39" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="42" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="42" customWidth="1"/>
+    <col min="3" max="3" width="18.6719" style="42" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="42" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="42" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="42" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="42" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="42" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="42" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="42" customWidth="1"/>
+    <col min="11" max="11" width="16.3516" style="42" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="42" customWidth="1"/>
+    <col min="13" max="13" width="16.3516" style="42" customWidth="1"/>
+    <col min="14" max="256" width="16.3516" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="40">
+      <c r="A1" t="s" s="43">
         <v>18</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" t="s" s="44">
-        <v>209</v>
-      </c>
-      <c r="B2" t="s" s="45">
-        <v>210</v>
-      </c>
-      <c r="C2" t="s" s="45">
-        <v>211</v>
-      </c>
-      <c r="D2" t="s" s="45">
+      <c r="A2" t="s" s="47">
         <v>212</v>
       </c>
-      <c r="E2" t="s" s="45">
+      <c r="B2" t="s" s="48">
         <v>213</v>
       </c>
-      <c r="F2" t="s" s="45">
+      <c r="C2" t="s" s="48">
         <v>214</v>
       </c>
-      <c r="G2" t="s" s="45">
+      <c r="D2" t="s" s="48">
         <v>215</v>
       </c>
-      <c r="H2" t="s" s="45">
+      <c r="E2" t="s" s="48">
         <v>216</v>
       </c>
-      <c r="I2" t="s" s="45">
+      <c r="F2" t="s" s="48">
         <v>217</v>
       </c>
-      <c r="J2" t="s" s="45">
+      <c r="G2" t="s" s="48">
         <v>218</v>
       </c>
-      <c r="K2" t="s" s="46">
+      <c r="H2" t="s" s="48">
         <v>219</v>
       </c>
-      <c r="L2" t="s" s="44">
+      <c r="I2" t="s" s="48">
         <v>220</v>
       </c>
-      <c r="M2" t="s" s="46">
+      <c r="J2" t="s" s="48">
         <v>221</v>
+      </c>
+      <c r="K2" t="s" s="49">
+        <v>222</v>
+      </c>
+      <c r="L2" t="s" s="47">
+        <v>223</v>
+      </c>
+      <c r="M2" t="s" s="49">
+        <v>224</v>
       </c>
     </row>
     <row r="3" ht="16.55" customHeight="1">
-      <c r="A3" t="s" s="47">
-        <v>222</v>
-      </c>
-      <c r="B3" t="s" s="23">
-        <v>223</v>
-      </c>
-      <c r="C3" t="s" s="48">
-        <v>224</v>
-      </c>
-      <c r="D3" s="49">
+      <c r="A3" t="s" s="50">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s" s="51">
+        <v>227</v>
+      </c>
+      <c r="D3" s="52">
         <v>12</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="52">
         <v>2022</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="52">
         <v>444</v>
       </c>
-      <c r="G3" t="s" s="24">
-        <v>225</v>
-      </c>
-      <c r="H3" t="s" s="24">
-        <v>226</v>
-      </c>
-      <c r="I3" s="49">
+      <c r="G3" t="s" s="27">
+        <v>228</v>
+      </c>
+      <c r="H3" t="s" s="27">
+        <v>229</v>
+      </c>
+      <c r="I3" s="52">
         <v>40</v>
       </c>
-      <c r="J3" s="49">
+      <c r="J3" s="52">
         <v>27</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="52">
         <v>15</v>
       </c>
-      <c r="L3" s="49">
+      <c r="L3" s="52">
         <v>22859882</v>
       </c>
-      <c r="M3" t="s" s="50">
-        <v>227</v>
+      <c r="M3" t="s" s="53">
+        <v>230</v>
       </c>
     </row>
     <row r="4" ht="16.35" customHeight="1">
-      <c r="A4" s="51"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="52"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="55"/>
     </row>
     <row r="5" ht="16.35" customHeight="1">
-      <c r="A5" s="51"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="52"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" ht="16.35" customHeight="1">
-      <c r="A6" s="51"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="52"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" ht="16.35" customHeight="1">
-      <c r="A7" s="51"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="52"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="55"/>
     </row>
     <row r="8" ht="16.35" customHeight="1">
-      <c r="A8" s="51"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="52"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" ht="16.35" customHeight="1">
-      <c r="A9" s="51"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="52"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" ht="16.35" customHeight="1">
-      <c r="A10" s="51"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="52"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="55"/>
     </row>
     <row r="11" ht="16.3" customHeight="1">
-      <c r="A11" s="54"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="57"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Dynamic creation of SOAP request elements using GoCompare and HomeConfused models
</commit_message>
<xml_diff>
--- a/AggregatorsData.xlsx
+++ b/AggregatorsData.xlsx
@@ -1727,14 +1727,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190338</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4347727</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>150721</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1743,7 +1743,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="1053938"/>
+          <a:off x="-19051" y="823660"/>
           <a:ext cx="4347728" cy="1765462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2324,15 +2324,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>467818</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>2960</xdr:rowOff>
+      <xdr:colOff>429716</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>596440</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>83273</xdr:rowOff>
+      <xdr:colOff>558338</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>14275</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2341,7 +2341,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1712418" y="1482510"/>
+          <a:off x="1674316" y="-980449"/>
           <a:ext cx="6351623" cy="18882684"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8583,14 +8583,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>118152</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>139334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>915952</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>90374</xdr:rowOff>
+      <xdr:colOff>992152</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>111555</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8599,8 +8599,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="2630212"/>
-          <a:ext cx="2160554" cy="1385732"/>
+          <a:off x="-19051" y="2449464"/>
+          <a:ext cx="2236754" cy="1385732"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9057,15 +9057,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>980440</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>155360</xdr:rowOff>
+      <xdr:colOff>942339</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1111716</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>14687</xdr:rowOff>
+      <xdr:colOff>1073614</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>6648</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9074,8 +9074,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225040" y="1219620"/>
-          <a:ext cx="6354276" cy="22913664"/>
+          <a:off x="2186938" y="-1494370"/>
+          <a:ext cx="6354277" cy="22913664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16696,14 +16696,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>68816</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>183342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>825369</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>133113</xdr:rowOff>
+      <xdr:rowOff>45709</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16712,8 +16712,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="2580876"/>
-          <a:ext cx="825370" cy="670088"/>
+          <a:off x="-19051" y="2493472"/>
+          <a:ext cx="825371" cy="670088"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>